<commit_message>
fixing matricula of Matc65
</commit_message>
<xml_diff>
--- a/build/ensino/2022/02/primeiro-semestre-de-2022/mes-3-dia-13-ava-matc65.xlsx
+++ b/build/ensino/2022/02/primeiro-semestre-de-2022/mes-3-dia-13-ava-matc65.xlsx
@@ -820,7 +820,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>216117974</t>
+          <t>217216526</t>
         </is>
       </c>
       <c r="B14">
@@ -854,7 +854,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>221117463</t>
+          <t>216117974</t>
         </is>
       </c>
       <c r="B15">
@@ -888,7 +888,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>219218129</t>
+          <t>221117463</t>
         </is>
       </c>
       <c r="B16">
@@ -922,7 +922,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>218215397</t>
+          <t>217125254</t>
         </is>
       </c>
       <c r="B17">
@@ -956,7 +956,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>217125254</t>
+          <t>219218129</t>
         </is>
       </c>
       <c r="B18">
@@ -990,7 +990,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>220117282</t>
+          <t>218215397</t>
         </is>
       </c>
       <c r="B19">
@@ -1024,7 +1024,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>219217429</t>
+          <t>220117282</t>
         </is>
       </c>
       <c r="B20">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>216216087</t>
+          <t>219217429</t>
         </is>
       </c>
       <c r="B21">
@@ -1092,7 +1092,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>220121412</t>
+          <t>216216087</t>
         </is>
       </c>
       <c r="B22">
@@ -1126,7 +1126,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>210201260</t>
+          <t>220121412</t>
         </is>
       </c>
       <c r="B23">
@@ -1160,7 +1160,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>201520233</t>
+          <t>210201260</t>
         </is>
       </c>
       <c r="B24">
@@ -1194,7 +1194,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>217117994</t>
+          <t>201520233</t>
         </is>
       </c>
       <c r="B25">
@@ -1228,7 +1228,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>219118481</t>
+          <t>217117994</t>
         </is>
       </c>
       <c r="B26">
@@ -1262,7 +1262,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>221119218</t>
+          <t>219118481</t>
         </is>
       </c>
       <c r="B27">
@@ -1296,7 +1296,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>219215012</t>
+          <t>221119218</t>
         </is>
       </c>
       <c r="B28">
@@ -1330,7 +1330,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>219121541</t>
+          <t>219215012</t>
         </is>
       </c>
       <c r="B29">
@@ -1364,7 +1364,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>214007731</t>
+          <t>219121541</t>
         </is>
       </c>
       <c r="B30">
@@ -1398,7 +1398,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>219215013</t>
+          <t>214007731</t>
         </is>
       </c>
       <c r="B31">
@@ -1432,7 +1432,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>220117290</t>
+          <t>219215013</t>
         </is>
       </c>
       <c r="B32">
@@ -1466,7 +1466,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>219118473</t>
+          <t>220117290</t>
         </is>
       </c>
       <c r="B33">
@@ -1500,7 +1500,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>220117273</t>
+          <t>219118473</t>
         </is>
       </c>
       <c r="B34">
@@ -1534,7 +1534,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>220120071</t>
+          <t>220117273</t>
         </is>
       </c>
       <c r="B35">
@@ -1568,7 +1568,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>221216783</t>
+          <t>220120071</t>
         </is>
       </c>
       <c r="B36">
@@ -1602,7 +1602,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>214120645</t>
+          <t>221216783</t>
         </is>
       </c>
       <c r="B37">
@@ -1636,7 +1636,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>220217140</t>
+          <t>214120645</t>
         </is>
       </c>
       <c r="B38">
@@ -1670,7 +1670,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>217117978</t>
+          <t>220217140</t>
         </is>
       </c>
       <c r="B39">

</xml_diff>